<commit_message>
added external_event table to the Engage tab of the sort variable spreadsheet since this was added to ENGAGEDIGITAL category as of schema 8
</commit_message>
<xml_diff>
--- a/ci360_database_table_sort_vars.xlsx
+++ b/ci360_database_table_sort_vars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\CI360_SAS_Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\github_respository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6D77D-7C1C-41F2-A580-AAED02BF6DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BABD849-4771-48D4-8F7D-F7152D4B4B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="420" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaIdent" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="186">
   <si>
     <t>EntityName</t>
   </si>
@@ -1460,7 +1460,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,13 +1822,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,6 +2190,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
     <sortCondition ref="A2:A32"/>

</xml_diff>

<commit_message>
modified the media table sort vars
</commit_message>
<xml_diff>
--- a/ci360_database_table_sort_vars.xlsx
+++ b/ci360_database_table_sort_vars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\github_respository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BABD849-4771-48D4-8F7D-F7152D4B4B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3788819B-54B4-4B43-A17C-57B946816E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaIdent" sheetId="5" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t xml:space="preserve">detail_id media_uri_txt action action_dttm </t>
   </si>
   <si>
-    <t>detail_id media_nm media_uri_txt interaction_cnt play_end_dttm</t>
-  </si>
-  <si>
     <t>md_activity_node</t>
   </si>
   <si>
@@ -595,6 +592,9 @@
   </si>
   <si>
     <t>notification_targeting_request</t>
+  </si>
+  <si>
+    <t>detail_id media_uri_txt play_end_dttm</t>
   </si>
 </sst>
 </file>
@@ -982,7 +982,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>48</v>
@@ -1012,16 +1012,16 @@
         <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -1030,25 +1030,25 @@
         <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -1057,25 +1057,25 @@
         <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="C12" s="7"/>
     </row>
@@ -1084,7 +1084,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="7"/>
     </row>
@@ -1093,16 +1093,16 @@
         <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="7"/>
     </row>
@@ -1111,16 +1111,16 @@
         <v>32</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="7"/>
     </row>
@@ -1129,7 +1129,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="7"/>
     </row>
@@ -1138,7 +1138,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="7"/>
     </row>
@@ -1147,34 +1147,34 @@
         <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="C23" s="7"/>
     </row>
@@ -1183,7 +1183,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="7"/>
     </row>
@@ -1192,7 +1192,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="7"/>
     </row>
@@ -1201,7 +1201,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" s="7"/>
     </row>
@@ -1210,25 +1210,25 @@
         <v>39</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="7"/>
     </row>
@@ -1237,13 +1237,13 @@
         <v>40</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>46</v>
@@ -1255,7 +1255,7 @@
         <v>41</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="7"/>
     </row>
@@ -1264,61 +1264,61 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="7"/>
     </row>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -1456,11 +1456,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B28:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -1527,10 +1527,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>23</v>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>23</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>47</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
@@ -1593,10 +1593,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>45</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>45</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>49</v>
@@ -1637,10 +1637,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>11</v>
@@ -1648,10 +1648,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>11</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>23</v>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>11</v>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>11</v>
@@ -1692,10 +1692,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>11</v>
@@ -1703,10 +1703,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>11</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>11</v>
@@ -1725,10 +1725,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>11</v>
@@ -1736,10 +1736,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>11</v>
@@ -1747,10 +1747,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>11</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>24</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>24</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>2</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>2</v>
@@ -1802,10 +1802,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>11</v>
@@ -1824,7 +1824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>44</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>44</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>44</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>44</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>44</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>44</v>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>44</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>44</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>44</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>44</v>
@@ -2016,7 +2016,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>44</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>44</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>44</v>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>44</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>44</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>44</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>44</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>44</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>44</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>44</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>44</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>11</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>44</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
added the remaining categories (plan, cdm, usage, abt) as additional tabs.  Changed the sort var list for the Engage tables to be more meaningful for most (vs. just using event_id).  Added in a couple new discover tables from schema 10.  Sort vars are in red for those that I have not tested/verified yet
</commit_message>
<xml_diff>
--- a/ci360_database_table_sort_vars.xlsx
+++ b/ci360_database_table_sort_vars.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\github_respository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3788819B-54B4-4B43-A17C-57B946816E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A8EF4B-BDBC-4611-BF6C-24A20AB8F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="2220" windowWidth="21600" windowHeight="11385" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaIdent" sheetId="5" r:id="rId1"/>
     <sheet name="Discover_Base" sheetId="3" r:id="rId2"/>
     <sheet name="Discover_Detail" sheetId="2" r:id="rId3"/>
     <sheet name="Engage" sheetId="4" r:id="rId4"/>
+    <sheet name="plan" sheetId="6" r:id="rId5"/>
+    <sheet name="cdm" sheetId="7" r:id="rId6"/>
+    <sheet name="usage" sheetId="8" r:id="rId7"/>
+    <sheet name="ABTs" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="345">
   <si>
     <t>EntityName</t>
   </si>
@@ -595,13 +599,490 @@
   </si>
   <si>
     <t>detail_id media_uri_txt play_end_dttm</t>
+  </si>
+  <si>
+    <t>cc_budget_breakup</t>
+  </si>
+  <si>
+    <t>cc_budget_breakup_ccbdgt</t>
+  </si>
+  <si>
+    <t>commitment_details</t>
+  </si>
+  <si>
+    <t>commitment_line_items</t>
+  </si>
+  <si>
+    <t>commitment_line_items_ccbdgt</t>
+  </si>
+  <si>
+    <t>fiscal_cc_budget</t>
+  </si>
+  <si>
+    <t>invoice_details</t>
+  </si>
+  <si>
+    <t>invoice_line_items</t>
+  </si>
+  <si>
+    <t>invoice_line_items_ccbdgt</t>
+  </si>
+  <si>
+    <t>md_bu</t>
+  </si>
+  <si>
+    <t>md_cost_category</t>
+  </si>
+  <si>
+    <t>md_costcenter</t>
+  </si>
+  <si>
+    <t>md_cust_attrib</t>
+  </si>
+  <si>
+    <t>md_custattrib_table_values</t>
+  </si>
+  <si>
+    <t>md_grid_attr_defn</t>
+  </si>
+  <si>
+    <t>md_fiscal_period</t>
+  </si>
+  <si>
+    <t>md_object_type</t>
+  </si>
+  <si>
+    <t>md_picklist</t>
+  </si>
+  <si>
+    <t>md_vendor</t>
+  </si>
+  <si>
+    <t>planning_hierarchy_defn</t>
+  </si>
+  <si>
+    <t>planning_info</t>
+  </si>
+  <si>
+    <t>planning_info_custom_prop</t>
+  </si>
+  <si>
+    <t>tag_details</t>
+  </si>
+  <si>
+    <t>asset_details</t>
+  </si>
+  <si>
+    <t>asset_details_custom_prop</t>
+  </si>
+  <si>
+    <t>asset_folder_details</t>
+  </si>
+  <si>
+    <t>asset_rendition_details</t>
+  </si>
+  <si>
+    <t>asset_revision</t>
+  </si>
+  <si>
+    <t>md_wf_process_def</t>
+  </si>
+  <si>
+    <t>md_wf_process_def_attr_grp</t>
+  </si>
+  <si>
+    <t>md_wf_process_def_categories</t>
+  </si>
+  <si>
+    <t>md_wf_process_def_task_assg</t>
+  </si>
+  <si>
+    <t>md_wf_process_def_tasks</t>
+  </si>
+  <si>
+    <t>wf_process_details</t>
+  </si>
+  <si>
+    <t>wf_process_details_custom_prop</t>
+  </si>
+  <si>
+    <t>wf_process_tasks</t>
+  </si>
+  <si>
+    <t>wf_tasks_user_assignment</t>
+  </si>
+  <si>
+    <t>asset_id</t>
+  </si>
+  <si>
+    <t>asset_id attr_id</t>
+  </si>
+  <si>
+    <t>planning_id attr_id</t>
+  </si>
+  <si>
+    <t>folder_id</t>
+  </si>
+  <si>
+    <t>rendition_id</t>
+  </si>
+  <si>
+    <t>revision_id</t>
+  </si>
+  <si>
+    <t>bu_id</t>
+  </si>
+  <si>
+    <t>vendor_id</t>
+  </si>
+  <si>
+    <t>planning_id</t>
+  </si>
+  <si>
+    <t>md_segment_test</t>
+  </si>
+  <si>
+    <t>md_segment_test_x_segment</t>
+  </si>
+  <si>
+    <t>abt_attribution</t>
+  </si>
+  <si>
+    <t>task_id task_version_id test_cd</t>
+  </si>
+  <si>
+    <t>task_id task_version_id segment_id test_cd</t>
+  </si>
+  <si>
+    <t>cost_center_id</t>
+  </si>
+  <si>
+    <t>cost_center_id fin_accnt_nm fp_id</t>
+  </si>
+  <si>
+    <t>planning_id cost_center_id fin_accnt_nm</t>
+  </si>
+  <si>
+    <t>planning_id cost_center_id fin_accnt_nm fp_id</t>
+  </si>
+  <si>
+    <t>planning_id cmtmnt_id vendor_id</t>
+  </si>
+  <si>
+    <t>planning_id cmtmnt_id vendor_id cost_center_id fin_acc_nm item_nm</t>
+  </si>
+  <si>
+    <t>planning_id cmtmnt_id vendor_id cost_center_id fin_acc_nm item_nm fp_id</t>
+  </si>
+  <si>
+    <t>planning_id cmtmnt_id invoice_id</t>
+  </si>
+  <si>
+    <t>planning_id cmtmnt_id invoice_id item_nm</t>
+  </si>
+  <si>
+    <t>planning_id cmtmnt_id invoice_id item_nm fp_id</t>
+  </si>
+  <si>
+    <t>ccat_id</t>
+  </si>
+  <si>
+    <t>attr_id</t>
+  </si>
+  <si>
+    <t>grid_id attr_id</t>
+  </si>
+  <si>
+    <t>fp_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attr_id </t>
+  </si>
+  <si>
+    <t>hier_defn_id level_nm</t>
+  </si>
+  <si>
+    <t>tag_id component_id</t>
+  </si>
+  <si>
+    <t>pdef_id version_num</t>
+  </si>
+  <si>
+    <t>pdef_id attr_group_id</t>
+  </si>
+  <si>
+    <t>pdef_id category_id</t>
+  </si>
+  <si>
+    <t>pdef_id task_id assignee_id</t>
+  </si>
+  <si>
+    <t>pdef_id task_id</t>
+  </si>
+  <si>
+    <t>process_id pdef_id process_instance_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">process_id attr_id </t>
+  </si>
+  <si>
+    <t>process_id task_id version_num instance_version</t>
+  </si>
+  <si>
+    <t>process_id task_id user_id user_assignment_id assignee_id</t>
+  </si>
+  <si>
+    <t>plist_id plist_cd attr_id</t>
+  </si>
+  <si>
+    <t>cdm_activity_custom_attr</t>
+  </si>
+  <si>
+    <t>cdm_activity_detail</t>
+  </si>
+  <si>
+    <t>cdm_activity_x_task</t>
+  </si>
+  <si>
+    <t>cdm_business_context</t>
+  </si>
+  <si>
+    <t>cdm_campaign_custom_attr</t>
+  </si>
+  <si>
+    <t>cdm_campaign_detail</t>
+  </si>
+  <si>
+    <t>cdm_dyn_content_custom_attr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdm_contact_channel </t>
+  </si>
+  <si>
+    <t>cdm_contact_history</t>
+  </si>
+  <si>
+    <t>cdm_contact_status</t>
+  </si>
+  <si>
+    <t>cdm_response_channel</t>
+  </si>
+  <si>
+    <t>cdm_response_extended_attr</t>
+  </si>
+  <si>
+    <t>cdm_response_history</t>
+  </si>
+  <si>
+    <t>cdm_response_lookup</t>
+  </si>
+  <si>
+    <t>cdm_response_type</t>
+  </si>
+  <si>
+    <t>cdm_content_custom_attr</t>
+  </si>
+  <si>
+    <t>cdm_content_detail</t>
+  </si>
+  <si>
+    <t>cdm_identifier_type</t>
+  </si>
+  <si>
+    <t>cdm_identity_attr</t>
+  </si>
+  <si>
+    <t>cdm_identity_map</t>
+  </si>
+  <si>
+    <t>cdm_identity_type</t>
+  </si>
+  <si>
+    <t>cdm_occurrence_detail</t>
+  </si>
+  <si>
+    <t>cdm_rtc_detail</t>
+  </si>
+  <si>
+    <t>cdm_rtc_x_content</t>
+  </si>
+  <si>
+    <t>cdm_segment_custom_attr</t>
+  </si>
+  <si>
+    <t>cdm_segment_detail</t>
+  </si>
+  <si>
+    <t>cdm_segment_map</t>
+  </si>
+  <si>
+    <t>cdm_segment_map_custom_attr</t>
+  </si>
+  <si>
+    <t>cdm_segment_test</t>
+  </si>
+  <si>
+    <t>cdm_segment_test_x_segment</t>
+  </si>
+  <si>
+    <t>cdm_task_custom_attr</t>
+  </si>
+  <si>
+    <t>cdm_task_detail</t>
+  </si>
+  <si>
+    <t>activity_id activity_version_id attribute_nm</t>
+  </si>
+  <si>
+    <t>content_id content_version_id attribute_nm</t>
+  </si>
+  <si>
+    <t>segment_id segment_version_id attribute_nm</t>
+  </si>
+  <si>
+    <t>segment_map_id segment_map_version_id attribute_nm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id attribute_nm</t>
+  </si>
+  <si>
+    <t>business_context_id</t>
+  </si>
+  <si>
+    <t>campaign_id page_nm attribute_nm</t>
+  </si>
+  <si>
+    <t>campaign_id campaign_version_no</t>
+  </si>
+  <si>
+    <t>content_id content_version_id attribute_nm content_hash_val</t>
+  </si>
+  <si>
+    <t>contact_channel_cd</t>
+  </si>
+  <si>
+    <t>contact_status_cd</t>
+  </si>
+  <si>
+    <t>response_channel_cd</t>
+  </si>
+  <si>
+    <t>response_type_cd</t>
+  </si>
+  <si>
+    <t>identity_type_cd</t>
+  </si>
+  <si>
+    <t>response_id attribute_nm</t>
+  </si>
+  <si>
+    <t>response_cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content_id content_version_id </t>
+  </si>
+  <si>
+    <t>identifier_type_id</t>
+  </si>
+  <si>
+    <t>daily_usage</t>
+  </si>
+  <si>
+    <t>monthly_usage</t>
+  </si>
+  <si>
+    <t>event_day</t>
+  </si>
+  <si>
+    <t>event_month</t>
+  </si>
+  <si>
+    <t>activity_id abtest_path_id identity_id</t>
+  </si>
+  <si>
+    <t>activity_id parent_event_designed_id identity_id activity_conversion_dttm</t>
+  </si>
+  <si>
+    <t>activity_id activity_node_id identity_id activity_flow_in_dttm</t>
+  </si>
+  <si>
+    <t>activity_id event_designed_id identity_id activity_start_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id parent_event_designed_id identity_id conversion_milestone_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id impression_delivered_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id impression_viewable_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id parent_event_designed_id identity_id response_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id parent_event_designed_id identity_id contact_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id spot_clicked_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id direct_contact_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id outbound_system_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_bounce_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_click_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_complaint_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_open_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_optout_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_action_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_reply_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_send_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id email_view_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id in_app_failed_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id event_designed_id identity_id in_app_failed_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id in_app_send_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id notification_failed_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id notification_opened_dttm</t>
+  </si>
+  <si>
+    <t>task_id task_version_id identity_id notification_send_dttm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +1103,19 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -650,7 +1144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -673,6 +1167,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,13 +1464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +1481,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1026,7 +1537,7 @@
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1053,7 +1564,7 @@
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1080,7 +1591,7 @@
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1089,7 +1600,7 @@
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1098,7 +1609,7 @@
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -1107,7 +1618,7 @@
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1116,7 +1627,7 @@
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1125,7 +1636,7 @@
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1134,7 +1645,7 @@
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1143,7 +1654,7 @@
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1152,7 +1663,7 @@
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1161,7 +1672,7 @@
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1170,7 +1681,7 @@
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -1179,7 +1690,7 @@
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -1188,7 +1699,7 @@
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -1197,7 +1708,7 @@
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1206,7 +1717,7 @@
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -1215,7 +1726,7 @@
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -1224,107 +1735,125 @@
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="7"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C41" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C39">
-    <sortCondition ref="A2:A39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C41">
+    <sortCondition ref="A2:A41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1336,7 +1865,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,11 +1988,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B28:B29"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,21 +2357,21 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1850,345 +2382,283 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>166</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>167</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>168</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>169</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>170</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>171</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>173</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>174</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>175</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>176</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>177</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>178</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
         <v>181</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>184</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="6" t="s">
         <v>164</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -2197,9 +2667,7 @@
       <c r="B33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C33" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
@@ -2208,4 +2676,786 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4817945-E189-427A-909E-EFDCC7DD3423}">
+  <dimension ref="A1:C38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>216</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>218</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>206</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3033CED8-6EC3-4A4D-8A86-DAEC2088785C}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>276</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>279</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>280</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>285</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>286</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>287</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>289</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>290</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>291</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>292</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>293</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" t="s">
+        <v>300</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>295</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFC424D-43B2-459B-BEAD-02BCB27B1C6C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA51031-1A03-434D-BBBD-F27B93179F77}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated sort vars for the CDM contact and response history tables
</commit_message>
<xml_diff>
--- a/ci360_database_table_sort_vars.xlsx
+++ b/ci360_database_table_sort_vars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\github_respository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A8EF4B-BDBC-4611-BF6C-24A20AB8F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9738DB-88D6-4226-B358-22D08DE292DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="2220" windowWidth="21600" windowHeight="11385" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1395" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaIdent" sheetId="5" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>md_task_custom_prop</t>
   </si>
   <si>
-    <t>contact_id</t>
-  </si>
-  <si>
     <t>event_id</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>impression_delivered</t>
   </si>
   <si>
-    <t>response_id</t>
-  </si>
-  <si>
     <t>activity_id activity_version_id</t>
   </si>
   <si>
@@ -1076,6 +1070,12 @@
   </si>
   <si>
     <t>task_id task_version_id identity_id notification_send_dttm</t>
+  </si>
+  <si>
+    <t>identity_id contact_dttm</t>
+  </si>
+  <si>
+    <t>identity_id response_dttm</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
@@ -1511,10 +1511,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -1523,16 +1523,16 @@
         <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -1541,25 +1541,25 @@
         <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -1568,25 +1568,25 @@
         <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="7"/>
     </row>
@@ -1595,7 +1595,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="7"/>
     </row>
@@ -1604,16 +1604,16 @@
         <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" s="7"/>
     </row>
@@ -1622,16 +1622,16 @@
         <v>32</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C17" s="7"/>
     </row>
@@ -1640,7 +1640,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C18" s="7"/>
     </row>
@@ -1649,7 +1649,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="7"/>
     </row>
@@ -1658,34 +1658,34 @@
         <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="C23" s="7"/>
     </row>
@@ -1694,7 +1694,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24" s="7"/>
     </row>
@@ -1703,7 +1703,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C25" s="7"/>
     </row>
@@ -1712,7 +1712,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C26" s="7"/>
     </row>
@@ -1721,43 +1721,43 @@
         <v>39</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" s="7"/>
     </row>
@@ -1766,16 +1766,16 @@
         <v>40</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="7"/>
     </row>
@@ -1784,7 +1784,7 @@
         <v>41</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C34" s="7"/>
     </row>
@@ -1793,61 +1793,61 @@
         <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C41" s="7"/>
     </row>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1900,7 +1900,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -2037,10 +2037,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -2059,10 +2059,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>23</v>
@@ -2081,10 +2081,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>23</v>
@@ -2103,10 +2103,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
@@ -2125,10 +2125,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>11</v>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>11</v>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>11</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>11</v>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>11</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>23</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>11</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>11</v>
@@ -2224,10 +2224,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>11</v>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>11</v>
@@ -2246,10 +2246,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>11</v>
@@ -2257,10 +2257,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>11</v>
@@ -2268,10 +2268,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>11</v>
@@ -2279,10 +2279,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>11</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>24</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>24</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>2</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>2</v>
@@ -2334,10 +2334,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>11</v>
@@ -2357,10 +2357,10 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C33"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,37 +2383,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -2422,7 +2422,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -2431,25 +2431,25 @@
         <v>16</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -2458,16 +2458,16 @@
         <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -2476,34 +2476,34 @@
         <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -2512,25 +2512,25 @@
         <v>22</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -2539,88 +2539,88 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -2629,16 +2629,16 @@
         <v>18</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -2647,22 +2647,22 @@
         <v>19</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>23</v>
@@ -2708,334 +2708,334 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C38" s="7"/>
     </row>
@@ -3049,11 +3049,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3033CED8-6EC3-4A4D-8A86-DAEC2088785C}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3076,169 +3076,169 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>343</v>
       </c>
       <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>64</v>
+        <v>344</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>26</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>25</v>
@@ -3256,109 +3256,109 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B32" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C33" s="7"/>
     </row>
@@ -3399,19 +3399,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" t="s">
         <v>314</v>
-      </c>
-      <c r="B2" t="s">
-        <v>316</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" t="s">
         <v>315</v>
-      </c>
-      <c r="B3" t="s">
-        <v>317</v>
       </c>
       <c r="C3" s="7"/>
     </row>
@@ -3424,7 +3424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA51031-1A03-434D-BBBD-F27B93179F77}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3451,7 +3451,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C2" s="7"/>
     </row>

</xml_diff>

<commit_message>
added md_task to the plan table sheet
</commit_message>
<xml_diff>
--- a/ci360_database_table_sort_vars.xlsx
+++ b/ci360_database_table_sort_vars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\github_respository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\github_repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9738DB-88D6-4226-B358-22D08DE292DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5AD0A8-C91D-4550-8B97-8461E0DBBF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaIdent" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="345">
   <si>
     <t>EntityName</t>
   </si>
@@ -1470,7 +1470,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2680,13 +2680,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4817945-E189-427A-909E-EFDCC7DD3423}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,130 +2914,139 @@
       <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>202</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>228</v>
+      <c r="A25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>212</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>252</v>
+        <v>202</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>228</v>
       </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>215</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>255</v>
+        <v>214</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>254</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>203</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>250</v>
+        <v>216</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>204</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>229</v>
+        <v>203</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>250</v>
       </c>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>217</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>257</v>
+        <v>206</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>251</v>
       </c>
       <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>220</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B39" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C39" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3049,7 +3058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3033CED8-6EC3-4A4D-8A86-DAEC2088785C}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>